<commit_message>
Update import specification abbreviations
</commit_message>
<xml_diff>
--- a/import-specification/devices/power-plant-controller.xlsx
+++ b/import-specification/devices/power-plant-controller.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>Field Type</t>
   </si>
@@ -179,6 +179,12 @@
     <t>Maximum active power during curtailment (3rd party)</t>
   </si>
   <si>
+    <t>PPC_P_SET_ABS</t>
+  </si>
+  <si>
+    <t>Absolute active power setpoint</t>
+  </si>
+  <si>
     <t>PPC_P_SET_GRIDOP_ABS</t>
   </si>
   <si>
@@ -194,10 +200,28 @@
     <t>Relative active power setpoint (grid operator)</t>
   </si>
   <si>
+    <t>PPC_P_SET_MANUAL_ABS</t>
+  </si>
+  <si>
+    <t>Absolute active power setpoint (manually)</t>
+  </si>
+  <si>
+    <t>PPC_P_SET_MANUAL_REL</t>
+  </si>
+  <si>
+    <t>Relative active power setpoint (manually)</t>
+  </si>
+  <si>
     <t>PPC_P_SET_REL</t>
   </si>
   <si>
     <t>Actual valid active power setpoint</t>
+  </si>
+  <si>
+    <t>PPC_P_SET_RPC_ABS</t>
+  </si>
+  <si>
+    <t>Absolute active power setpoint (3rd party)</t>
   </si>
   <si>
     <t>PPC_P_SET_RPC_REL</t>
@@ -581,7 +605,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,10 +931,10 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
         <v>57</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -918,17 +942,14 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
         <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
       </c>
       <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
@@ -938,7 +959,7 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
@@ -952,10 +973,10 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
         <v>64</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -963,13 +984,16 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
         <v>66</v>
       </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
+      <c r="F23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -977,13 +1001,13 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
         <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -991,13 +1015,69 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
         <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new abbreviations for PPC device
</commit_message>
<xml_diff>
--- a/import-specification/devices/power-plant-controller.xlsx
+++ b/import-specification/devices/power-plant-controller.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
   <si>
     <t>Field Type</t>
   </si>
@@ -287,6 +287,12 @@
     <t>Relative active power setpoint (manually)</t>
   </si>
   <si>
+    <t>PPC_P_SET_MODE</t>
+  </si>
+  <si>
+    <t>Active power control method  0: No configuration found 1: Variable fixed value Pvar fix 2: Variable fixed value Pvar DI 3: Variable fixed value Pvar AI 4: Variable fixed value Pvar Modbus 5: Remote Power Control (RPC) 100: LFSM-O 101: LFSM-U 102: FSM 112: RPC (Remote Power Control) &amp; FSM 200: Fail-safe operation (hold last setpoint) 201: Fail-safe operation (default setpoint) 202: Fail-safe operation (system fallback value) 203: Fail-safe operation (Automatic grid disconnection)</t>
+  </si>
+  <si>
     <t>PPC_P_SET_REL</t>
   </si>
   <si>
@@ -335,10 +341,25 @@
     <t>Absolute reactive power setpoint</t>
   </si>
   <si>
+    <t>PPC_Q_SET_MODE</t>
+  </si>
+  <si>
+    <t>Reactive power control method  0: No configuration found 1: Variable fixed value cos φvar fix 2: Variable fixed value cos φvar DI 3: Variable fixed value cos φvar AI 4: Variable fixed value cos φvar Modbus 5: Characteristic curve cos φ (P) 6: Characteristic curve cos φ (V) 7: Variable fixed value Qvar fix 8: Variable fixed value Qvar DI 9: Variable fixed value Qvar AI 10: Variable fixed value Qvar Modbus 11: Characteristic curve Q (P) 12: Characteristic curve Q (V) 13: Characteristic curve Q (tan φ) 14: Voltage control Q (V droop) 15: Characteristic curve Q(V) Modbus, from firmware 28.0.2 on 16: Characteristic curve cos φ (P) Modbus, from firmware 28.0.2 on 100: Reactive power compensation 200: Fail-safe operation (hold last setpoint) 201: Fail-safe operation (default setpoint) 202: Fail-safe operation (system fallback value)</t>
+  </si>
+  <si>
     <t>PPC_Q_SET_REL</t>
   </si>
   <si>
     <t>Reactive power setpoint</t>
+  </si>
+  <si>
+    <t>PPC_V_REF_Q_V_SHIFT</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Voltage shift for Q(V) curve</t>
   </si>
   <si>
     <t>STATE[1..x]</t>
@@ -696,7 +717,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,7 +728,7 @@
     <col min="1" max="1" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="65.984" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="988.473" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="54.13" bestFit="true" customWidth="true" style="0"/>
@@ -1239,15 +1260,9 @@
       <c r="B35" t="s">
         <v>90</v>
       </c>
-      <c r="C35" t="s">
-        <v>45</v>
-      </c>
       <c r="D35" t="s">
         <v>91</v>
       </c>
-      <c r="F35" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
@@ -1257,11 +1272,14 @@
         <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
         <v>93</v>
       </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
@@ -1271,7 +1289,7 @@
         <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D37" t="s">
         <v>95</v>
@@ -1285,7 +1303,7 @@
         <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
         <v>97</v>
@@ -1299,7 +1317,7 @@
         <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
         <v>99</v>
@@ -1313,7 +1331,7 @@
         <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
         <v>101</v>
@@ -1355,7 +1373,7 @@
         <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
         <v>107</v>
@@ -1370,6 +1388,45 @@
       </c>
       <c r="D44" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D47" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>